<commit_message>
update all documents 2024-07-11
</commit_message>
<xml_diff>
--- a/RegistraBOT_ws/src/database_RegistraBOT/raw_catalogo/raw_catalogo_productos.xlsx
+++ b/RegistraBOT_ws/src/database_RegistraBOT/raw_catalogo/raw_catalogo_productos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="79">
   <si>
     <t>sku</t>
   </si>
@@ -46,7 +46,7 @@
     <t>Granel</t>
   </si>
   <si>
-    <t>Cebolla</t>
+    <t>Verdura</t>
   </si>
   <si>
     <t>Bolsa Plástico</t>
@@ -55,7 +55,7 @@
     <t>Cebolla Morada</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/GR-VR-BS-GRA-000-001.png</t>
+    <t>database_RegistraBOT/product_images/GR-VR-BS-GRA-000-001.png</t>
   </si>
   <si>
     <t>GR-VR-BS-GRA-000-002</t>
@@ -64,31 +64,28 @@
     <t>Cebolla Blanca</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/GR-VR-BS-GRA-000-002.png</t>
+    <t>database_RegistraBOT/product_images/GR-VR-BS-GRA-000-002.png</t>
   </si>
   <si>
     <t>GR-FR-BS-GRA-000-001</t>
   </si>
   <si>
-    <t>Platano</t>
+    <t>Fruta</t>
   </si>
   <si>
     <t>Plátano Seda</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/GR-FR-BS-GRA-000-001.png</t>
+    <t>database_RegistraBOT/product_images/GR-FR-BS-GRA-000-001.png</t>
   </si>
   <si>
     <t>GR-VR-BS-GRA-000-003</t>
   </si>
   <si>
-    <t>Papa</t>
-  </si>
-  <si>
     <t>Papa Amarilla</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/GR-VR-BS-GRA-000-003.png</t>
+    <t>database_RegistraBOT/product_images/GR-VR-BS-GRA-000-003.png</t>
   </si>
   <si>
     <t>GR-VR-BS-GRA-000-004</t>
@@ -97,7 +94,7 @@
     <t>Papa Blanca</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/GR-VR-BS-GRA-000-004.png</t>
+    <t>database_RegistraBOT/product_images/GR-VR-BS-GRA-000-004.png</t>
   </si>
   <si>
     <t>GR-VR-BS-GRA-000-005</t>
@@ -106,7 +103,7 @@
     <t>Papa Huayro</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/GR-VR-BS-GRA-000-005.png</t>
+    <t>database_RegistraBOT/product_images/GR-VR-BS-GRA-000-005.png</t>
   </si>
   <si>
     <t>GR-VR-BS-GRA-000-006</t>
@@ -115,7 +112,7 @@
     <t>Papa Blanca Chilena</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/GR-VR-BS-GRA-000-006.png</t>
+    <t>database_RegistraBOT/product_images/GR-VR-BS-GRA-000-006.png</t>
   </si>
   <si>
     <t>LC-LE-TP-GLO-001-001</t>
@@ -139,7 +136,7 @@
     <t>Leche Gloria Entera</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/LC-LE-TP-GLO-001-001.png</t>
+    <t>database_RegistraBOT/product_images/LC-LE-TP-GLO-001-001.png</t>
   </si>
   <si>
     <t>AB-MY-DP-ALA-475-001</t>
@@ -163,7 +160,7 @@
     <t>Mayonesa Alacena</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/AB-MY-DP-ALA-475-001.png</t>
+    <t>database_RegistraBOT/product_images/AB-MY-DP-ALA-475-001.png</t>
   </si>
   <si>
     <t>AB-CR-DP-ALA-400-001</t>
@@ -178,7 +175,7 @@
     <t>Uchucuta Alacena</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/AB-CR-DP-ALA-400-001.png</t>
+    <t>database_RegistraBOT/product_images/AB-CR-DP-ALA-400-001.png</t>
   </si>
   <si>
     <t>AB-CO-BS-AJI-250-001</t>
@@ -196,7 +193,7 @@
     <t>Sazonador Ajinomoto</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/AB-CO-BS-AJI-250-001.png</t>
+    <t>database_RegistraBOT/product_images/AB-CO-BS-AJI-250-001.png</t>
   </si>
   <si>
     <t>LP-LT-BP-POE-900-001</t>
@@ -220,7 +217,7 @@
     <t>Poett Lavanda</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/LP-LT-BP-POE-900-001.png</t>
+    <t>database_RegistraBOT/product_images/LP-LT-BP-POE-900-001.png</t>
   </si>
   <si>
     <t>LP-DE-FP-NIV-050-001</t>
@@ -241,7 +238,7 @@
     <t>Deso Hombre Invisible B&amp;W</t>
   </si>
   <si>
-    <t>/src/database_RegistraBOT/product_images/LP-DE-FP-NIV-050-001.png</t>
+    <t>database_RegistraBOT/product_images/LP-DE-FP-NIV-050-001.png</t>
   </si>
   <si>
     <t>ND-ND-ND-ND-000-000</t>
@@ -318,13 +315,13 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,7 +585,7 @@
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -597,7 +594,7 @@
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>0.0</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -606,7 +603,7 @@
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -617,7 +614,7 @@
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -626,7 +623,7 @@
       <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>0.0</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -635,7 +632,7 @@
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -646,7 +643,7 @@
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -655,7 +652,7 @@
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <v>0.0</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -664,7 +661,7 @@
       <c r="H4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -675,8 +672,8 @@
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -684,28 +681,28 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <v>0.0</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -713,28 +710,28 @@
       <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <v>0.0</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -742,28 +739,28 @@
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <v>0.0</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -771,220 +768,220 @@
       <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>0.0</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="4">
+        <v>475.0</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="3">
-        <v>475.0</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="4">
+        <v>400.0</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="3">
-        <v>400.0</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="4">
+        <v>250.0</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="3">
-        <v>250.0</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="4">
+        <v>900.0</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="3">
-        <v>900.0</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="4">
+        <v>50.0</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="3">
-        <v>50.0</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="I15" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>